<commit_message>
Finished the second revision of the review on improvement objectives and technical problems addressed by BC-IoT prototypes. Finished extracting data for RQ2 and RQ3 of upto 45 papers, closes #27, closes #21.
</commit_message>
<xml_diff>
--- a/DataExtraction/Extracted Data/RQ2_RQ3/extraction_Q2_Q3_v0.1.1.xlsx
+++ b/DataExtraction/Extracted Data/RQ2_RQ3/extraction_Q2_Q3_v0.1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trannguyen/Documents/CodeProjects/BC-IoT_SLR/BC_IoT_SLR/DataExtraction/Extracted Data/RQ2_RQ3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0564EA-BC55-5848-A1B1-EBBB2984B4D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FF0C90-9948-2549-8299-5866E0E5938F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="994" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2106" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2200" uniqueCount="414">
   <si>
     <t>Paper ID</t>
   </si>
@@ -1248,6 +1248,40 @@
   </si>
   <si>
     <t>Sensor Reading Hashes</t>
+  </si>
+  <si>
+    <t>Data placement records; Resource exchange records</t>
+  </si>
+  <si>
+    <t>Device Authentication; Public Key Infrastructure; Data registry; Business process orchestrator</t>
+  </si>
+  <si>
+    <t>Cryptographic keys generation; Device Authentication</t>
+  </si>
+  <si>
+    <t>bitcoin</t>
+  </si>
+  <si>
+    <t>Trust management system
+	Trust rating record</t>
+  </si>
+  <si>
+    <t>Sensor Reading Hashes; Device descriptions; Resource exchange records</t>
+  </si>
+  <si>
+    <t>Device, Data, and Service Authorisation;Data registry; Business process orchestrator</t>
+  </si>
+  <si>
+    <t>consortium</t>
+  </si>
+  <si>
+    <t>Joint PoW PoS</t>
+  </si>
+  <si>
+    <t>in-house BC system</t>
+  </si>
+  <si>
+    <t>Business process orchestrator; Trust management system</t>
   </si>
 </sst>
 </file>
@@ -1742,9 +1776,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G48" sqref="G48"/>
+      <selection pane="topRight" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2336,8 +2370,12 @@
       <c r="E29" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
+      <c r="F29" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
@@ -2752,7 +2790,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>142</v>
       </c>
@@ -2768,8 +2806,12 @@
       <c r="E49" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
+      <c r="F49" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
@@ -2787,8 +2829,12 @@
       <c r="E50" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
+      <c r="F50" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
@@ -2913,8 +2959,12 @@
       <c r="E56" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
+      <c r="F56" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="57" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
@@ -3314,8 +3364,12 @@
       <c r="E75" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F75" s="6"/>
-      <c r="G75" s="6"/>
+      <c r="F75" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="76" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
@@ -3543,8 +3597,12 @@
       <c r="E86" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F86" s="6"/>
-      <c r="G86" s="6"/>
+      <c r="F86" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="87" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
@@ -3659,9 +3717,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319240B9-4870-494A-A276-E36B79402EDE}">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F48" sqref="F48"/>
+      <selection pane="topRight" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4265,6 +4323,21 @@
       <c r="E29" t="s">
         <v>8</v>
       </c>
+      <c r="F29" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="30" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
@@ -4815,8 +4888,23 @@
       <c r="E49" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="F49" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>145</v>
       </c>
@@ -4831,6 +4919,21 @@
       </c>
       <c r="E50" t="s">
         <v>12</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -4970,6 +5073,21 @@
       <c r="E56" t="s">
         <v>12</v>
       </c>
+      <c r="F56" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J56" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="57" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
@@ -5431,6 +5549,21 @@
       <c r="E75" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F75" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I75" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J75" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="76" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
@@ -5692,6 +5825,21 @@
       </c>
       <c r="E86" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I86" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="J86" s="6" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="64" x14ac:dyDescent="0.2">
@@ -5819,9 +5967,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3962EE67-A2B1-0B49-9F74-9CC75A10F5DD}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L48" sqref="L48"/>
+      <selection pane="topRight" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6494,6 +6642,30 @@
       <c r="E29" t="s">
         <v>8</v>
       </c>
+      <c r="F29" s="6">
+        <v>2</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="30" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
@@ -7170,6 +7342,30 @@
       <c r="E49" t="s">
         <v>12</v>
       </c>
+      <c r="F49" s="6">
+        <v>1</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="L49" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M49" s="6" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="50" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
@@ -7187,6 +7383,30 @@
       <c r="E50" t="s">
         <v>12</v>
       </c>
+      <c r="F50" s="6">
+        <v>1</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K50" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="L50" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M50" s="6" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="51" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
@@ -7361,6 +7581,30 @@
       <c r="E56" t="s">
         <v>12</v>
       </c>
+      <c r="F56" s="6">
+        <v>1</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="J56" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K56" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="L56" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M56" s="6" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="57" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
@@ -7924,6 +8168,30 @@
       <c r="E75" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F75" s="6">
+        <v>1</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I75" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="J75" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K75" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L75" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M75" s="6" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="76" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
@@ -8230,6 +8498,30 @@
       </c>
       <c r="E86" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="F86" s="6">
+        <v>1</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I86" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J86" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="K86" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L86" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M86" s="6" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="112" x14ac:dyDescent="0.2">
@@ -8375,9 +8667,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DCB22C-FF00-B845-92DB-3CB3C377A5B2}">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F42" sqref="F1:F1048576"/>
+      <selection pane="topRight" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8924,6 +9216,12 @@
       <c r="E29" t="s">
         <v>8</v>
       </c>
+      <c r="F29" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
@@ -9342,6 +9640,12 @@
       <c r="E49" t="s">
         <v>12</v>
       </c>
+      <c r="F49" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
@@ -9479,6 +9783,12 @@
       <c r="E56" t="s">
         <v>12</v>
       </c>
+      <c r="F56" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="57" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
@@ -9862,6 +10172,12 @@
       <c r="E75" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F75" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="76" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
@@ -10078,6 +10394,12 @@
       </c>
       <c r="E86" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="112" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Extracted data for RQ2 and RQ3 upto 55 papers.
</commit_message>
<xml_diff>
--- a/DataExtraction/Extracted Data/RQ2_RQ3/extraction_Q2_Q3_v0.1.1.xlsx
+++ b/DataExtraction/Extracted Data/RQ2_RQ3/extraction_Q2_Q3_v0.1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trannguyen/Documents/CodeProjects/BC-IoT_SLR/BC_IoT_SLR/DataExtraction/Extracted Data/RQ2_RQ3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FF0C90-9948-2549-8299-5866E0E5938F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B84A6DC-F7FF-B24A-9CD4-21AD4CD9A326}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="994" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2200" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2376" uniqueCount="431">
   <si>
     <t>Paper ID</t>
   </si>
@@ -1282,6 +1282,57 @@
   </si>
   <si>
     <t>Business process orchestrator; Trust management system</t>
+  </si>
+  <si>
+    <t>Proof-of-stake</t>
+  </si>
+  <si>
+    <t>Communication channel; Device, Data, and Service Authorisation; Device Authentication</t>
+  </si>
+  <si>
+    <t>Sensor Data Storage; Business process orchestrator</t>
+  </si>
+  <si>
+    <t>Blockchain PoW consumes too much energy for IoT use cases.</t>
+  </si>
+  <si>
+    <t>Selective Proof-of-work</t>
+  </si>
+  <si>
+    <t>Commands to devices</t>
+  </si>
+  <si>
+    <t>Command integrity check</t>
+  </si>
+  <si>
+    <t>Resource exchange records; Service interaction records</t>
+  </si>
+  <si>
+    <t>Contract between resource providers and consumers; Service Matchmaking mechanism</t>
+  </si>
+  <si>
+    <t>Device, Data, and Service Authorisation; Interaction and incident record</t>
+  </si>
+  <si>
+    <t>Trail prediction</t>
+  </si>
+  <si>
+    <t>Digital Twins of IoT devices</t>
+  </si>
+  <si>
+    <t>Sensor Data Storage; Publish-Subscribe middleware</t>
+  </si>
+  <si>
+    <t>Publish-subscribe protocol</t>
+  </si>
+  <si>
+    <t>Sensor Data Storage; Trust management system</t>
+  </si>
+  <si>
+    <t>Authorisation mechanism; Contract between resource providers and consumers</t>
+  </si>
+  <si>
+    <t>Proof-of-work; Proof-of-space</t>
   </si>
 </sst>
 </file>
@@ -1776,9 +1827,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G30" sqref="G30"/>
+      <selection pane="topRight" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2208,8 +2259,12 @@
       <c r="E21" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
+      <c r="F21" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
@@ -2332,8 +2387,12 @@
       <c r="E27" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
+      <c r="F27" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
@@ -2477,8 +2536,12 @@
       <c r="E34" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
+      <c r="F34" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
@@ -2630,8 +2693,12 @@
       <c r="E41" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
+      <c r="F41" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
@@ -2718,8 +2785,12 @@
       <c r="E45" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
+      <c r="F45" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
@@ -3062,8 +3133,12 @@
       <c r="E61" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F61" s="6"/>
-      <c r="G61" s="6"/>
+      <c r="F61" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="62" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
@@ -3165,8 +3240,12 @@
       <c r="E66" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F66" s="6"/>
-      <c r="G66" s="6"/>
+      <c r="F66" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="67" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
@@ -3184,8 +3263,12 @@
       <c r="E67" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F67" s="6"/>
-      <c r="G67" s="6"/>
+      <c r="F67" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="68" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
@@ -3456,8 +3539,12 @@
       <c r="E79" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F79" s="6"/>
-      <c r="G79" s="6"/>
+      <c r="F79" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="80" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
@@ -3643,8 +3730,12 @@
       <c r="E88" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F88" s="6"/>
-      <c r="G88" s="6"/>
+      <c r="F88" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="89" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="10" t="s">
@@ -3662,8 +3753,12 @@
       <c r="E89" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F89" s="6"/>
-      <c r="G89" s="6"/>
+      <c r="F89" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="G89" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="90" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A90" s="10" t="s">
@@ -3717,9 +3812,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319240B9-4870-494A-A276-E36B79402EDE}">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G30" sqref="G30"/>
+      <selection pane="topRight" activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4157,6 +4252,21 @@
       <c r="E21" t="s">
         <v>8</v>
       </c>
+      <c r="F21" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="22" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -4289,6 +4399,21 @@
       <c r="E27" t="s">
         <v>8</v>
       </c>
+      <c r="F27" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="28" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
@@ -4468,6 +4593,21 @@
       <c r="E34" t="s">
         <v>12</v>
       </c>
+      <c r="F34" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="35" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
@@ -4662,6 +4802,21 @@
       <c r="E41" t="s">
         <v>23</v>
       </c>
+      <c r="F41" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="42" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
@@ -4759,7 +4914,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>131</v>
       </c>
@@ -4774,6 +4929,21 @@
       </c>
       <c r="E45" t="s">
         <v>12</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="80" x14ac:dyDescent="0.2">
@@ -5185,6 +5355,21 @@
       <c r="E61" t="s">
         <v>12</v>
       </c>
+      <c r="F61" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H61" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J61" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="62" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
@@ -5300,6 +5485,21 @@
       <c r="E66" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F66" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="67" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
@@ -5317,6 +5517,21 @@
       <c r="E67" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F67" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J67" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="68" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
@@ -5677,6 +5892,21 @@
       <c r="E79" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F79" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H79" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I79" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J79" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="80" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
@@ -5874,7 +6104,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>246</v>
       </c>
@@ -5890,8 +6120,23 @@
       <c r="E88" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="F88" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H88" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="I88" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J88" s="6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>249</v>
       </c>
@@ -5906,6 +6151,21 @@
       </c>
       <c r="E89" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="G89" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H89" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="I89" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J89" s="6" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="80" x14ac:dyDescent="0.2">
@@ -5967,9 +6227,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3962EE67-A2B1-0B49-9F74-9CC75A10F5DD}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H30" sqref="H30"/>
+      <selection pane="topRight" activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6458,6 +6718,30 @@
       <c r="E21" t="s">
         <v>8</v>
       </c>
+      <c r="F21" s="6">
+        <v>1</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="22" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -6608,6 +6892,30 @@
       <c r="E27" t="s">
         <v>8</v>
       </c>
+      <c r="F27" s="6">
+        <v>1</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="28" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
@@ -6823,6 +7131,30 @@
       <c r="E34" t="s">
         <v>12</v>
       </c>
+      <c r="F34" s="6">
+        <v>1</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="35" spans="1:13" ht="160" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
@@ -7062,6 +7394,30 @@
       <c r="E41" t="s">
         <v>23</v>
       </c>
+      <c r="F41" s="6">
+        <v>1</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M41" s="6" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="42" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
@@ -7202,6 +7558,30 @@
       <c r="E45" t="s">
         <v>12</v>
       </c>
+      <c r="F45" s="6">
+        <v>1</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="L45" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M45" s="6" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="46" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
@@ -7714,6 +8094,30 @@
       <c r="E61" t="s">
         <v>12</v>
       </c>
+      <c r="F61" s="6">
+        <v>1</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H61" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="J61" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="K61" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L61" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M61" s="6" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="62" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
@@ -7847,6 +8251,30 @@
       <c r="E66" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F66" s="6">
+        <v>1</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K66" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L66" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M66" s="6" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="67" spans="1:13" ht="112" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
@@ -7864,6 +8292,30 @@
       <c r="E67" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F67" s="6">
+        <v>1</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="J67" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K67" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L67" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M67" s="6" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="68" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
@@ -8332,6 +8784,30 @@
       <c r="E79" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F79" s="6">
+        <v>4</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H79" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I79" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J79" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K79" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L79" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M79" s="6" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="80" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
@@ -8581,6 +9057,30 @@
       <c r="E88" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F88" s="6">
+        <v>1</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H88" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I88" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="J88" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K88" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="L88" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M88" s="6" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="89" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
@@ -8597,6 +9097,30 @@
       </c>
       <c r="E89" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="F89" s="6">
+        <v>1</v>
+      </c>
+      <c r="G89" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H89" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I89" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="J89" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K89" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L89" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M89" s="6" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="90" spans="1:13" ht="64" x14ac:dyDescent="0.2">
@@ -8667,9 +9191,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DCB22C-FF00-B845-92DB-3CB3C377A5B2}">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F30" sqref="F30"/>
+      <selection pane="topRight" activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9068,6 +9592,12 @@
       <c r="E21" t="s">
         <v>8</v>
       </c>
+      <c r="F21" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -9182,6 +9712,12 @@
       <c r="E27" t="s">
         <v>8</v>
       </c>
+      <c r="F27" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
@@ -9319,6 +9855,12 @@
       <c r="E34" t="s">
         <v>12</v>
       </c>
+      <c r="F34" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
@@ -9468,6 +10010,12 @@
       <c r="E41" t="s">
         <v>23</v>
       </c>
+      <c r="F41" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
@@ -9554,6 +10102,12 @@
       <c r="E45" t="s">
         <v>12</v>
       </c>
+      <c r="F45" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
@@ -9880,6 +10434,12 @@
       <c r="E61" t="s">
         <v>12</v>
       </c>
+      <c r="F61" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>414</v>
+      </c>
     </row>
     <row r="62" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
@@ -9977,6 +10537,12 @@
       <c r="E66" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F66" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="67" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
@@ -9994,6 +10560,12 @@
       <c r="E67" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F67" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="68" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
@@ -10264,6 +10836,12 @@
       <c r="E79" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F79" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="80" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
@@ -10441,6 +11019,12 @@
       <c r="E88" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F88" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="89" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
@@ -10457,6 +11041,12 @@
       </c>
       <c r="E89" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G89" s="6" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="64" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Extracted data for RQ2 and RQ3 upto 65 papers. Closes #28. Closes #22
</commit_message>
<xml_diff>
--- a/DataExtraction/Extracted Data/RQ2_RQ3/extraction_Q2_Q3_v0.1.1.xlsx
+++ b/DataExtraction/Extracted Data/RQ2_RQ3/extraction_Q2_Q3_v0.1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trannguyen/Documents/CodeProjects/BC-IoT_SLR/BC_IoT_SLR/DataExtraction/Extracted Data/RQ2_RQ3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B84A6DC-F7FF-B24A-9CD4-21AD4CD9A326}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C235DE55-02FC-4A42-B40E-5C6E01EB8A32}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="994" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2376" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2519" uniqueCount="444">
   <si>
     <t>Paper ID</t>
   </si>
@@ -1198,9 +1198,6 @@
     <t>Digital-twin of devices</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Business process orchestrator; Digital Twins of IoT devices</t>
   </si>
   <si>
@@ -1333,6 +1330,48 @@
   </si>
   <si>
     <t>Proof-of-work; Proof-of-space</t>
+  </si>
+  <si>
+    <t>Filter data before writing to the chain</t>
+  </si>
+  <si>
+    <t>Access control</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Public &amp; Private</t>
+  </si>
+  <si>
+    <t>IoT injects too many transactions at too high rate into blockchains; Blockchain PoW consumes too much energy for IoT use cases.</t>
+  </si>
+  <si>
+    <t>Replace PoW with distributed trust</t>
+  </si>
+  <si>
+    <t>Sensor Reading Hashes; Authorisation policies</t>
+  </si>
+  <si>
+    <t>n/A</t>
+  </si>
+  <si>
+    <t>Sensor Reading Hashes; Firmware Hash</t>
+  </si>
+  <si>
+    <t>Eris</t>
+  </si>
+  <si>
+    <t>Sensor Reading Hashes; Authorisation requests and responses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device, Data, and Service Authorisation </t>
+  </si>
+  <si>
+    <t>Cloud; Edge</t>
+  </si>
+  <si>
+    <t>Resource exchange records; Service descriptions</t>
   </si>
 </sst>
 </file>
@@ -1827,9 +1866,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G46" sqref="G46"/>
+      <selection pane="topRight" activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2027,8 +2066,12 @@
       <c r="E9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
@@ -2179,8 +2222,12 @@
       <c r="E17" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="F17" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
@@ -2198,8 +2245,12 @@
       <c r="E18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
+      <c r="F18" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
@@ -2260,7 +2311,7 @@
         <v>8</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>270</v>
@@ -2283,9 +2334,11 @@
         <v>8</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="G22" s="6"/>
+        <v>441</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
@@ -2303,8 +2356,12 @@
       <c r="E23" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
+      <c r="F23" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
@@ -2322,8 +2379,12 @@
       <c r="E24" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
+      <c r="F24" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
@@ -2388,7 +2449,7 @@
         <v>8</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>288</v>
@@ -2430,7 +2491,7 @@
         <v>8</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>288</v>
@@ -2476,10 +2537,10 @@
         <v>8</v>
       </c>
       <c r="F31" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="G31" s="6" t="s">
         <v>387</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -2694,7 +2755,7 @@
         <v>23</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>288</v>
@@ -2740,7 +2801,7 @@
         <v>8</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>288</v>
@@ -2786,7 +2847,7 @@
         <v>12</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>288</v>
@@ -2809,7 +2870,7 @@
         <v>8</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>332</v>
@@ -2832,7 +2893,7 @@
         <v>8</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>288</v>
@@ -2878,7 +2939,7 @@
         <v>12</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>288</v>
@@ -2901,7 +2962,7 @@
         <v>12</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>288</v>
@@ -3053,8 +3114,12 @@
       <c r="E57" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
+      <c r="F57" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="58" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
@@ -3218,7 +3283,7 @@
         <v>12</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G65" s="6" t="s">
         <v>288</v>
@@ -3241,7 +3306,7 @@
         <v>8</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G66" s="6" t="s">
         <v>288</v>
@@ -3264,7 +3329,7 @@
         <v>8</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G67" s="6" t="s">
         <v>288</v>
@@ -3287,7 +3352,7 @@
         <v>23</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G68" s="6" t="s">
         <v>288</v>
@@ -3379,7 +3444,7 @@
         <v>12</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G72" s="6" t="s">
         <v>269</v>
@@ -3448,7 +3513,7 @@
         <v>8</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G75" s="6" t="s">
         <v>270</v>
@@ -3540,7 +3605,7 @@
         <v>12</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G79" s="6" t="s">
         <v>288</v>
@@ -3581,8 +3646,12 @@
       <c r="E81" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F81" s="6"/>
-      <c r="G81" s="6"/>
+      <c r="F81" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="82" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A82" s="10" t="s">
@@ -3600,8 +3669,12 @@
       <c r="E82" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F82" s="6"/>
-      <c r="G82" s="6"/>
+      <c r="F82" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="83" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
@@ -3731,7 +3804,7 @@
         <v>12</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G88" s="6" t="s">
         <v>288</v>
@@ -3812,9 +3885,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319240B9-4870-494A-A276-E36B79402EDE}">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I46" sqref="I46"/>
+      <selection pane="topRight" activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4036,6 +4109,21 @@
       <c r="E9" t="s">
         <v>8</v>
       </c>
+      <c r="F9" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -4172,6 +4260,21 @@
       <c r="E17" t="s">
         <v>23</v>
       </c>
+      <c r="F17" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
@@ -4189,6 +4292,21 @@
       <c r="E18" t="s">
         <v>8</v>
       </c>
+      <c r="F18" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="19" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
@@ -4265,7 +4383,7 @@
         <v>271</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -4284,6 +4402,21 @@
       <c r="E22" t="s">
         <v>8</v>
       </c>
+      <c r="F22" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="23" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
@@ -4301,6 +4434,21 @@
       <c r="E23" t="s">
         <v>12</v>
       </c>
+      <c r="F23" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="24" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
@@ -4318,6 +4466,21 @@
       <c r="E24" t="s">
         <v>8</v>
       </c>
+      <c r="F24" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="25" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
@@ -4594,13 +4757,13 @@
         <v>12</v>
       </c>
       <c r="F34" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H34" s="6" t="s">
         <v>419</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>420</v>
       </c>
       <c r="I34" s="6" t="s">
         <v>271</v>
@@ -4867,7 +5030,7 @@
         <v>8</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>271</v>
@@ -4937,7 +5100,7 @@
         <v>271</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I45" s="6" t="s">
         <v>271</v>
@@ -4995,7 +5158,7 @@
         <v>8</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>271</v>
@@ -5059,7 +5222,7 @@
         <v>12</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>306</v>
@@ -5068,7 +5231,7 @@
         <v>271</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J49" s="6" t="s">
         <v>271</v>
@@ -5091,7 +5254,7 @@
         <v>12</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>271</v>
@@ -5275,6 +5438,21 @@
       <c r="E57" t="s">
         <v>8</v>
       </c>
+      <c r="F57" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="I57" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J57" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="58" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
@@ -5518,13 +5696,13 @@
         <v>8</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G67" s="6" t="s">
         <v>271</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I67" s="6" t="s">
         <v>271</v>
@@ -5550,16 +5728,16 @@
         <v>23</v>
       </c>
       <c r="F68" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H68" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="G68" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="H68" s="6" t="s">
+      <c r="I68" s="6" t="s">
         <v>398</v>
-      </c>
-      <c r="I68" s="6" t="s">
-        <v>399</v>
       </c>
       <c r="J68" s="6" t="s">
         <v>271</v>
@@ -5941,6 +6119,21 @@
       <c r="E81" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F81" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H81" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I81" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J81" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="82" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
@@ -5958,6 +6151,21 @@
       <c r="E82" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F82" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H82" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I82" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J82" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="83" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
@@ -6121,13 +6329,13 @@
         <v>12</v>
       </c>
       <c r="F88" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H88" s="6" t="s">
         <v>421</v>
-      </c>
-      <c r="G88" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="H88" s="6" t="s">
-        <v>422</v>
       </c>
       <c r="I88" s="6" t="s">
         <v>271</v>
@@ -6227,9 +6435,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3962EE67-A2B1-0B49-9F74-9CC75A10F5DD}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M46" sqref="M46"/>
+      <selection pane="topRight" activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6490,6 +6698,30 @@
       <c r="E9" t="s">
         <v>8</v>
       </c>
+      <c r="F9" s="6">
+        <v>2</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="112" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -6626,6 +6858,30 @@
       <c r="E17" t="s">
         <v>23</v>
       </c>
+      <c r="F17" s="6">
+        <v>1</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="18" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
@@ -6643,6 +6899,30 @@
       <c r="E18" t="s">
         <v>8</v>
       </c>
+      <c r="F18" s="6">
+        <v>1</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="19" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
@@ -6759,6 +7039,30 @@
       <c r="E22" t="s">
         <v>8</v>
       </c>
+      <c r="F22" s="6">
+        <v>1</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="23" spans="1:13" ht="112" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
@@ -6776,6 +7080,30 @@
       <c r="E23" t="s">
         <v>12</v>
       </c>
+      <c r="F23" s="6">
+        <v>1</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="24" spans="1:13" ht="112" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
@@ -6793,6 +7121,30 @@
       <c r="E24" t="s">
         <v>8</v>
       </c>
+      <c r="F24" s="6">
+        <v>1</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="25" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
@@ -7571,7 +7923,7 @@
         <v>300</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K45" s="6" t="s">
         <v>302</v>
@@ -7744,7 +8096,7 @@
         <v>271</v>
       </c>
       <c r="M49" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="64" x14ac:dyDescent="0.2">
@@ -7779,7 +8131,7 @@
         <v>293</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="L50" s="6" t="s">
         <v>271</v>
@@ -8002,6 +8354,30 @@
       <c r="E57" t="s">
         <v>8</v>
       </c>
+      <c r="F57" s="6">
+        <v>1</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I57" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="J57" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="K57" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="L57" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M57" s="6" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="58" spans="1:13" ht="112" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
@@ -8107,7 +8483,7 @@
         <v>275</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="K61" s="6" t="s">
         <v>281</v>
@@ -8346,7 +8722,7 @@
         <v>300</v>
       </c>
       <c r="J68" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K68" s="6" t="s">
         <v>302</v>
@@ -8355,7 +8731,7 @@
         <v>271</v>
       </c>
       <c r="M68" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="69" spans="1:13" ht="64" x14ac:dyDescent="0.2">
@@ -8842,6 +9218,30 @@
       <c r="E81" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F81" s="6">
+        <v>1</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H81" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I81" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J81" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="K81" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="L81" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M81" s="6" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="82" spans="1:13" ht="112" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
@@ -8859,6 +9259,30 @@
       <c r="E82" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F82" s="6">
+        <v>1</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H82" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I82" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="J82" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="K82" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="L82" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M82" s="6" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="83" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
@@ -8988,7 +9412,7 @@
         <v>271</v>
       </c>
       <c r="J86" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="K86" s="6" t="s">
         <v>281</v>
@@ -8997,7 +9421,7 @@
         <v>271</v>
       </c>
       <c r="M86" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="112" x14ac:dyDescent="0.2">
@@ -9191,9 +9615,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DCB22C-FF00-B845-92DB-3CB3C377A5B2}">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F42" sqref="F42"/>
+      <selection pane="topRight" activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9382,6 +9806,12 @@
       <c r="E9" t="s">
         <v>8</v>
       </c>
+      <c r="F9" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -9518,6 +9948,12 @@
       <c r="E17" t="s">
         <v>23</v>
       </c>
+      <c r="F17" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
@@ -9535,6 +9971,12 @@
       <c r="E18" t="s">
         <v>8</v>
       </c>
+      <c r="F18" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>430</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
@@ -9615,6 +10057,12 @@
       <c r="E22" t="s">
         <v>8</v>
       </c>
+      <c r="F22" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
@@ -9632,6 +10080,12 @@
       <c r="E23" t="s">
         <v>12</v>
       </c>
+      <c r="F23" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
@@ -9649,6 +10103,12 @@
       <c r="E24" t="s">
         <v>8</v>
       </c>
+      <c r="F24" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
@@ -9802,7 +10262,7 @@
         <v>320</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -10360,6 +10820,12 @@
       <c r="E57" t="s">
         <v>8</v>
       </c>
+      <c r="F57" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="58" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
@@ -10438,7 +10904,7 @@
         <v>322</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="48" x14ac:dyDescent="0.2">
@@ -10837,10 +11303,10 @@
         <v>12</v>
       </c>
       <c r="F79" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="G79" s="6" t="s">
         <v>417</v>
-      </c>
-      <c r="G79" s="6" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -10876,6 +11342,12 @@
       <c r="E81" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F81" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="82" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
@@ -10892,6 +11364,12 @@
       </c>
       <c r="E82" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="32" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Extracted data for RQ2 and RQ3 up to 76 papers out of 90. Closes #23. Closes #29
</commit_message>
<xml_diff>
--- a/DataExtraction/Extracted Data/RQ2_RQ3/extraction_Q2_Q3_v0.1.1.xlsx
+++ b/DataExtraction/Extracted Data/RQ2_RQ3/extraction_Q2_Q3_v0.1.1.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trannguyen/Documents/CodeProjects/BC-IoT_SLR/BC_IoT_SLR/DataExtraction/Extracted Data/RQ2_RQ3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trannguyen/Documents/CodeProjects/BC_IoT_SLR/DataExtraction/Extracted Data/RQ2_RQ3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C235DE55-02FC-4A42-B40E-5C6E01EB8A32}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B76D95-305A-C448-9590-9E1CDEA34D61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="994" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="994" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RQ2.1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2519" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2675" uniqueCount="454">
   <si>
     <t>Paper ID</t>
   </si>
@@ -1148,10 +1148,6 @@
     <t>Sensor Readings; Service interaction records</t>
   </si>
   <si>
-    <t>Service descriptions;
-Device descriptions</t>
-  </si>
-  <si>
     <t>Service interaction records; Device interaction records</t>
   </si>
   <si>
@@ -1263,9 +1259,6 @@
 	Trust rating record</t>
   </si>
   <si>
-    <t>Sensor Reading Hashes; Device descriptions; Resource exchange records</t>
-  </si>
-  <si>
     <t>Device, Data, and Service Authorisation;Data registry; Business process orchestrator</t>
   </si>
   <si>
@@ -1341,9 +1334,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>Public &amp; Private</t>
-  </si>
-  <si>
     <t>IoT injects too many transactions at too high rate into blockchains; Blockchain PoW consumes too much energy for IoT use cases.</t>
   </si>
   <si>
@@ -1356,9 +1346,6 @@
     <t>n/A</t>
   </si>
   <si>
-    <t>Sensor Reading Hashes; Firmware Hash</t>
-  </si>
-  <si>
     <t>Eris</t>
   </si>
   <si>
@@ -1372,6 +1359,49 @@
   </si>
   <si>
     <t>Resource exchange records; Service descriptions</t>
+  </si>
+  <si>
+    <t>Data index maintenance</t>
+  </si>
+  <si>
+    <t>Sensor Readings; Device configurations; Device interaction records</t>
+  </si>
+  <si>
+    <t>more than 2</t>
+  </si>
+  <si>
+    <t>Firmware Delivery</t>
+  </si>
+  <si>
+    <t>Firmware Hash (and Binary)</t>
+  </si>
+  <si>
+    <t>Sensor Reading Hashes; Firmware Hash (and Binary)</t>
+  </si>
+  <si>
+    <t>Aggregate data before writing to the chain</t>
+  </si>
+  <si>
+    <t>Commands to devices; Sensor Reading Hashes</t>
+  </si>
+  <si>
+    <t>Devices might generate transactions without owners’ approval</t>
+  </si>
+  <si>
+    <t>Integrate owners’ biometrics into the signature used by devices</t>
+  </si>
+  <si>
+    <t>Identity Management System</t>
+  </si>
+  <si>
+    <t>Sensor Reading Hashes; Device description and identitys; Resource exchange records</t>
+  </si>
+  <si>
+    <t>Service descriptions;
+Device description and identitys</t>
+  </si>
+  <si>
+    <t>Device description and identity</t>
   </si>
 </sst>
 </file>
@@ -1866,9 +1896,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G58" sqref="G58"/>
+      <selection pane="topRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1944,8 +1974,12 @@
       <c r="E3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -2028,8 +2062,12 @@
       <c r="E7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
@@ -2047,8 +2085,12 @@
       <c r="E8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
@@ -2089,8 +2131,12 @@
       <c r="E10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
@@ -2127,8 +2173,12 @@
       <c r="E12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
@@ -2146,8 +2196,12 @@
       <c r="E13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
@@ -2165,8 +2219,12 @@
       <c r="E14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
@@ -2184,8 +2242,12 @@
       <c r="E15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
@@ -2203,8 +2265,12 @@
       <c r="E16" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
@@ -2246,7 +2312,7 @@
         <v>8</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>288</v>
@@ -2268,8 +2334,12 @@
       <c r="E19" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="F19" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
@@ -2311,7 +2381,7 @@
         <v>8</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>270</v>
@@ -2334,7 +2404,7 @@
         <v>8</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>288</v>
@@ -2360,7 +2430,7 @@
         <v>366</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -2449,7 +2519,7 @@
         <v>8</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>288</v>
@@ -2491,7 +2561,7 @@
         <v>8</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>288</v>
@@ -2537,10 +2607,10 @@
         <v>8</v>
       </c>
       <c r="F31" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="G31" s="6" t="s">
         <v>386</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -2755,7 +2825,7 @@
         <v>23</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>288</v>
@@ -2801,7 +2871,7 @@
         <v>8</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>288</v>
@@ -2847,7 +2917,7 @@
         <v>12</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>288</v>
@@ -2870,7 +2940,7 @@
         <v>8</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>332</v>
@@ -2893,7 +2963,7 @@
         <v>8</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>288</v>
@@ -2939,7 +3009,7 @@
         <v>12</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>288</v>
@@ -2962,7 +3032,7 @@
         <v>12</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>288</v>
@@ -3115,7 +3185,7 @@
         <v>8</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>288</v>
@@ -3140,9 +3210,7 @@
       <c r="F58" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="G58" s="6" t="s">
-        <v>288</v>
-      </c>
+      <c r="G58" s="6"/>
     </row>
     <row r="59" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
@@ -3283,7 +3351,7 @@
         <v>12</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G65" s="6" t="s">
         <v>288</v>
@@ -3306,7 +3374,7 @@
         <v>8</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G66" s="6" t="s">
         <v>288</v>
@@ -3329,7 +3397,7 @@
         <v>8</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G67" s="6" t="s">
         <v>288</v>
@@ -3352,7 +3420,7 @@
         <v>23</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G68" s="6" t="s">
         <v>288</v>
@@ -3444,7 +3512,7 @@
         <v>12</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G72" s="6" t="s">
         <v>269</v>
@@ -3513,7 +3581,7 @@
         <v>8</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G75" s="6" t="s">
         <v>270</v>
@@ -3559,7 +3627,7 @@
         <v>8</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G77" s="6" t="s">
         <v>288</v>
@@ -3605,7 +3673,7 @@
         <v>12</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="G79" s="6" t="s">
         <v>288</v>
@@ -3804,7 +3872,7 @@
         <v>12</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G88" s="6" t="s">
         <v>288</v>
@@ -3885,9 +3953,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319240B9-4870-494A-A276-E36B79402EDE}">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I58" sqref="I58"/>
+      <selection pane="topRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3949,19 +4017,19 @@
         <v>8</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>376</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -3980,6 +4048,21 @@
       <c r="E3" t="s">
         <v>12</v>
       </c>
+      <c r="F3" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -4030,7 +4113,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>296</v>
@@ -4075,6 +4158,21 @@
       <c r="E7" t="s">
         <v>23</v>
       </c>
+      <c r="F7" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -4092,6 +4190,21 @@
       <c r="E8" t="s">
         <v>8</v>
       </c>
+      <c r="F8" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -4110,7 +4223,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>271</v>
@@ -4122,7 +4235,7 @@
         <v>271</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="80" x14ac:dyDescent="0.2">
@@ -4141,6 +4254,21 @@
       <c r="E10" t="s">
         <v>12</v>
       </c>
+      <c r="F10" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -4159,7 +4287,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
@@ -4174,6 +4302,21 @@
       </c>
       <c r="E12" t="s">
         <v>8</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -4192,6 +4335,21 @@
       <c r="E13" t="s">
         <v>8</v>
       </c>
+      <c r="F13" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -4209,6 +4367,21 @@
       <c r="E14" t="s">
         <v>8</v>
       </c>
+      <c r="F14" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -4226,6 +4399,21 @@
       <c r="E15" t="s">
         <v>8</v>
       </c>
+      <c r="F15" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -4243,6 +4431,21 @@
       <c r="E16" t="s">
         <v>8</v>
       </c>
+      <c r="F16" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -4261,13 +4464,13 @@
         <v>23</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>271</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>271</v>
@@ -4324,6 +4527,21 @@
       <c r="E19" t="s">
         <v>8</v>
       </c>
+      <c r="F19" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="20" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
@@ -4348,7 +4566,7 @@
         <v>271</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>307</v>
@@ -4371,7 +4589,7 @@
         <v>8</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>271</v>
@@ -4383,7 +4601,7 @@
         <v>271</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -4435,7 +4653,7 @@
         <v>12</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>271</v>
@@ -4467,7 +4685,7 @@
         <v>8</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>271</v>
@@ -4499,7 +4717,7 @@
         <v>12</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>271</v>
@@ -4531,13 +4749,13 @@
         <v>12</v>
       </c>
       <c r="F26" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H26" s="6" t="s">
         <v>384</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>385</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>271</v>
@@ -4563,13 +4781,13 @@
         <v>8</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>271</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>271</v>
@@ -4612,7 +4830,7 @@
         <v>8</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>271</v>
@@ -4676,13 +4894,13 @@
         <v>8</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>271</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I31" s="6" t="s">
         <v>271</v>
@@ -4757,13 +4975,13 @@
         <v>12</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>271</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="I34" s="6" t="s">
         <v>271</v>
@@ -4821,16 +5039,16 @@
         <v>8</v>
       </c>
       <c r="F36" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I36" s="6" t="s">
         <v>382</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>383</v>
       </c>
       <c r="J36" s="6" t="s">
         <v>271</v>
@@ -4902,7 +5120,7 @@
         <v>8</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>271</v>
@@ -4966,7 +5184,7 @@
         <v>23</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>271</v>
@@ -5030,7 +5248,7 @@
         <v>8</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>271</v>
@@ -5100,7 +5318,7 @@
         <v>271</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="I45" s="6" t="s">
         <v>271</v>
@@ -5158,7 +5376,7 @@
         <v>8</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>271</v>
@@ -5222,7 +5440,7 @@
         <v>12</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>306</v>
@@ -5231,7 +5449,7 @@
         <v>271</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J49" s="6" t="s">
         <v>271</v>
@@ -5254,7 +5472,7 @@
         <v>12</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>407</v>
+        <v>451</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>271</v>
@@ -5303,7 +5521,7 @@
         <v>8</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>271</v>
@@ -5439,7 +5657,7 @@
         <v>8</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>271</v>
@@ -5600,7 +5818,7 @@
         <v>12</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G64" s="6" t="s">
         <v>271</v>
@@ -5632,7 +5850,7 @@
         <v>12</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>370</v>
+        <v>452</v>
       </c>
       <c r="G65" s="6" t="s">
         <v>271</v>
@@ -5696,13 +5914,13 @@
         <v>8</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G67" s="6" t="s">
         <v>271</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="I67" s="6" t="s">
         <v>271</v>
@@ -5728,16 +5946,16 @@
         <v>23</v>
       </c>
       <c r="F68" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H68" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G68" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="H68" s="6" t="s">
+      <c r="I68" s="6" t="s">
         <v>397</v>
-      </c>
-      <c r="I68" s="6" t="s">
-        <v>398</v>
       </c>
       <c r="J68" s="6" t="s">
         <v>271</v>
@@ -6007,13 +6225,13 @@
         <v>8</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G77" s="6" t="s">
         <v>271</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I77" s="6" t="s">
         <v>271</v>
@@ -6120,7 +6338,7 @@
         <v>8</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
       <c r="G81" s="6" t="s">
         <v>271</v>
@@ -6152,7 +6370,7 @@
         <v>8</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G82" s="6" t="s">
         <v>271</v>
@@ -6329,13 +6547,13 @@
         <v>12</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="G88" s="6" t="s">
         <v>271</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="I88" s="6" t="s">
         <v>271</v>
@@ -6435,9 +6653,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3962EE67-A2B1-0B49-9F74-9CC75A10F5DD}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J58" sqref="J58"/>
+      <selection pane="topRight" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6529,7 +6747,7 @@
         <v>271</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="64" x14ac:dyDescent="0.2">
@@ -6548,6 +6766,30 @@
       <c r="E3" t="s">
         <v>12</v>
       </c>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -6664,6 +6906,30 @@
       <c r="E7" t="s">
         <v>23</v>
       </c>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -6681,6 +6947,30 @@
       <c r="E8" t="s">
         <v>8</v>
       </c>
+      <c r="F8" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="128" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -6711,10 +7001,10 @@
         <v>271</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>433</v>
+        <v>395</v>
       </c>
       <c r="L9" s="6" t="s">
         <v>271</v>
@@ -6739,6 +7029,30 @@
       <c r="E10" t="s">
         <v>12</v>
       </c>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -6773,6 +7087,30 @@
       <c r="E12" t="s">
         <v>8</v>
       </c>
+      <c r="F12" s="6">
+        <v>1</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -6790,6 +7128,30 @@
       <c r="E13" t="s">
         <v>8</v>
       </c>
+      <c r="F13" s="6">
+        <v>1</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -6807,6 +7169,30 @@
       <c r="E14" t="s">
         <v>8</v>
       </c>
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="15" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -6824,6 +7210,30 @@
       <c r="E15" t="s">
         <v>8</v>
       </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -6841,6 +7251,30 @@
       <c r="E16" t="s">
         <v>8</v>
       </c>
+      <c r="F16" s="6">
+        <v>1</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="17" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -6940,6 +7374,30 @@
       <c r="E19" t="s">
         <v>8</v>
       </c>
+      <c r="F19" s="6">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="20" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
@@ -7923,7 +8381,7 @@
         <v>300</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K45" s="6" t="s">
         <v>302</v>
@@ -8096,7 +8554,7 @@
         <v>271</v>
       </c>
       <c r="M49" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="64" x14ac:dyDescent="0.2">
@@ -8131,7 +8589,7 @@
         <v>293</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="L50" s="6" t="s">
         <v>271</v>
@@ -8370,7 +8828,7 @@
         <v>301</v>
       </c>
       <c r="K57" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="L57" s="6" t="s">
         <v>271</v>
@@ -8483,7 +8941,7 @@
         <v>275</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="K61" s="6" t="s">
         <v>281</v>
@@ -8722,7 +9180,7 @@
         <v>300</v>
       </c>
       <c r="J68" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K68" s="6" t="s">
         <v>302</v>
@@ -8731,7 +9189,7 @@
         <v>271</v>
       </c>
       <c r="M68" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="69" spans="1:13" ht="64" x14ac:dyDescent="0.2">
@@ -9094,7 +9552,7 @@
         <v>293</v>
       </c>
       <c r="K77" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="L77" s="6" t="s">
         <v>271</v>
@@ -9272,7 +9730,7 @@
         <v>275</v>
       </c>
       <c r="J82" s="6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="K82" s="6" t="s">
         <v>304</v>
@@ -9281,7 +9739,7 @@
         <v>271</v>
       </c>
       <c r="M82" s="6" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="32" x14ac:dyDescent="0.2">
@@ -9412,7 +9870,7 @@
         <v>271</v>
       </c>
       <c r="J86" s="6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="K86" s="6" t="s">
         <v>281</v>
@@ -9421,7 +9879,7 @@
         <v>271</v>
       </c>
       <c r="M86" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="112" x14ac:dyDescent="0.2">
@@ -9615,9 +10073,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DCB22C-FF00-B845-92DB-3CB3C377A5B2}">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E56" sqref="E56"/>
+      <selection pane="topRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9772,6 +10230,12 @@
       <c r="E7" t="s">
         <v>23</v>
       </c>
+      <c r="F7" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -9789,6 +10253,12 @@
       <c r="E8" t="s">
         <v>8</v>
       </c>
+      <c r="F8" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -9807,10 +10277,10 @@
         <v>8</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -9829,6 +10299,12 @@
       <c r="E10" t="s">
         <v>12</v>
       </c>
+      <c r="F10" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>449</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -9863,6 +10339,12 @@
       <c r="E12" t="s">
         <v>8</v>
       </c>
+      <c r="F12" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -9897,6 +10379,12 @@
       <c r="E14" t="s">
         <v>8</v>
       </c>
+      <c r="F14" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -9914,6 +10402,12 @@
       <c r="E15" t="s">
         <v>8</v>
       </c>
+      <c r="F15" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -9931,6 +10425,12 @@
       <c r="E16" t="s">
         <v>8</v>
       </c>
+      <c r="F16" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -9975,7 +10475,7 @@
         <v>322</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -9994,6 +10494,12 @@
       <c r="E19" t="s">
         <v>8</v>
       </c>
+      <c r="F19" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
@@ -10262,7 +10768,7 @@
         <v>320</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="112" x14ac:dyDescent="0.2">
@@ -10904,7 +11410,7 @@
         <v>322</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="48" x14ac:dyDescent="0.2">
@@ -11303,10 +11809,10 @@
         <v>12</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="64" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Recommit with the updated spreadsheet.
</commit_message>
<xml_diff>
--- a/DataExtraction/Extracted Data/RQ2_RQ3/extraction_Q2_Q3_v0.1.1.xlsx
+++ b/DataExtraction/Extracted Data/RQ2_RQ3/extraction_Q2_Q3_v0.1.1.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trannguyen/Documents/CodeProjects/BC_IoT_SLR/DataExtraction/Extracted Data/RQ2_RQ3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B76D95-305A-C448-9590-9E1CDEA34D61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768C4C4A-C57C-F645-A47A-B2467D417520}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="994" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RQ2.1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2675" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2679" uniqueCount="454">
   <si>
     <t>Paper ID</t>
   </si>
@@ -1896,9 +1896,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G20" sqref="G20"/>
+      <selection pane="topRight" activeCell="F7" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3953,9 +3953,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319240B9-4870-494A-A276-E36B79402EDE}">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G20" sqref="G20"/>
+      <selection pane="topRight" activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10073,9 +10073,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DCB22C-FF00-B845-92DB-3CB3C377A5B2}">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F20" sqref="F20"/>
+      <selection pane="topRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10150,6 +10150,12 @@
       <c r="E3" t="s">
         <v>12</v>
       </c>
+      <c r="F3" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -10361,6 +10367,12 @@
       </c>
       <c r="E13" t="s">
         <v>8</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="80" x14ac:dyDescent="0.2">

</xml_diff>